<commit_message>
Fix the initial set-up of the rest of the scripts before focusing on Fig. 5E
</commit_message>
<xml_diff>
--- a/data/Other/excelSheet/Fig5/Fig5BCF.xlsx
+++ b/data/Other/excelSheet/Fig5/Fig5BCF.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>Row</t>
   </si>
@@ -140,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -150,14 +150,18 @@
     </border>
     <border/>
     <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -190,60 +194,60 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -296,7 +300,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
@@ -349,7 +353,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -402,7 +406,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5">
@@ -455,7 +459,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B6">
@@ -508,7 +512,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B7">
@@ -561,7 +565,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8">
@@ -614,7 +618,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9">
@@ -667,7 +671,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B10">
@@ -720,7 +724,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B11">
@@ -773,7 +777,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B12">
@@ -826,7 +830,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B13">
@@ -879,7 +883,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14">
@@ -932,7 +936,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B15">
@@ -985,7 +989,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B16">
@@ -1038,7 +1042,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B17">
@@ -1091,7 +1095,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B18">
@@ -1144,7 +1148,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B19">

</xml_diff>